<commit_message>
Added try-except case to fix issues with values
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -769,17 +769,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>40/40</t>
+          <t>40</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HP</t>
+          <t>40</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9885</t>
+          <t>Defense</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">

</xml_diff>

<commit_message>
Added data overwriting functionality to the spreadsheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="units" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -67,13 +67,13 @@
     <t>Beth</t>
   </si>
   <si>
-    <t>shamann</t>
-  </si>
-  <si>
-    <t>astar</t>
-  </si>
-  <si>
-    <t>teo</t>
+    <t>Shamann</t>
+  </si>
+  <si>
+    <t>Astar</t>
+  </si>
+  <si>
+    <t>Teo</t>
   </si>
   <si>
     <t>Kyle</t>
@@ -91,7 +91,7 @@
     <t>Bellenus</t>
   </si>
   <si>
-    <t>tushen</t>
+    <t>Tushen</t>
   </si>
   <si>
     <t>Emma</t>

</xml_diff>